<commit_message>
Fixed grade for tp
</commit_message>
<xml_diff>
--- a/Doc/TestPlan/TP-Rubrics.xlsx
+++ b/Doc/TestPlan/TP-Rubrics.xlsx
@@ -574,8 +574,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:C36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -845,7 +845,7 @@
         <v>24</v>
       </c>
       <c r="B29" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C29" s="4">
         <v>2</v>
@@ -856,7 +856,7 @@
         <v>25</v>
       </c>
       <c r="B30" s="4">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C30" s="4">
         <v>5</v>
@@ -912,7 +912,7 @@
       </c>
       <c r="B35" s="6">
         <f>SUM(B17:B34)</f>
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="C35" s="6">
         <v>70</v>
@@ -924,7 +924,7 @@
       </c>
       <c r="B36" s="13">
         <f>SUM(B35,B14,B10,B6)</f>
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="C36" s="13">
         <v>100</v>

</xml_diff>